<commit_message>
Rajout Fichier html character
</commit_message>
<xml_diff>
--- a/docs/Monstres.xlsx
+++ b/docs/Monstres.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33840" windowHeight="21940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16960" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Monster" sheetId="1" r:id="rId1"/>
+    <sheet name="Classe" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>Frondon</t>
   </si>
@@ -124,6 +125,24 @@
   </si>
   <si>
     <t>Gain Xp</t>
+  </si>
+  <si>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>Orque</t>
+  </si>
+  <si>
+    <t>Gobelin</t>
+  </si>
+  <si>
+    <t>UrukHaï</t>
+  </si>
+  <si>
+    <t>RoiSorcier</t>
+  </si>
+  <si>
+    <t>Troll</t>
   </si>
 </sst>
 </file>
@@ -172,8 +191,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -182,11 +203,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -789,4 +812,85 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="8" max="8" width="19.625" customWidth="1"/>
+    <col min="10" max="10" width="19.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>